<commit_message>
Fixed some color values
</commit_message>
<xml_diff>
--- a/src/assets/colors.xlsx
+++ b/src/assets/colors.xlsx
@@ -305,22 +305,22 @@
     <t>1129FF</t>
   </si>
   <si>
-    <t>1580FF</t>
-  </si>
-  <si>
-    <t>1363FF</t>
-  </si>
-  <si>
-    <t>8272FF</t>
-  </si>
-  <si>
-    <t>7365FF</t>
-  </si>
-  <si>
-    <t>5850FF</t>
-  </si>
-  <si>
-    <t>8770FF</t>
+    <t>001580</t>
+  </si>
+  <si>
+    <t>001363</t>
+  </si>
+  <si>
+    <t>008272</t>
+  </si>
+  <si>
+    <t>007365</t>
+  </si>
+  <si>
+    <t>005850</t>
+  </si>
+  <si>
+    <t>008770</t>
   </si>
 </sst>
 </file>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3570,43 +3570,43 @@
       </c>
       <c r="B65" t="str">
         <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C65" t="str">
-        <f t="shared" si="1"/>
+      <c r="D65" t="str">
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="D65" t="str">
-        <f t="shared" si="2"/>
-        <v>FF</v>
-      </c>
       <c r="E65">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="F65">
-        <f t="shared" si="4"/>
+      <c r="G65">
+        <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="G65">
-        <f t="shared" si="5"/>
-        <v>255</v>
-      </c>
       <c r="H65">
         <f t="shared" si="6"/>
-        <v>404</v>
+        <v>149</v>
       </c>
       <c r="I65" t="str">
         <f t="shared" si="7"/>
-        <v>light</v>
+        <v>dark</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="8"/>
-        <v>000000</v>
+        <v>FFFFFF</v>
       </c>
       <c r="K65" t="str">
         <f t="shared" si="9"/>
-        <v>{"background": "#1580FF", "foreground": "#000000"}</v>
+        <v>{"background": "#001580", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -3615,31 +3615,31 @@
       </c>
       <c r="B66" t="str">
         <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C66" t="str">
-        <f t="shared" si="1"/>
+      <c r="D66" t="str">
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="D66" t="str">
-        <f t="shared" si="2"/>
-        <v>FF</v>
-      </c>
       <c r="E66">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="F66">
-        <f t="shared" si="4"/>
+      <c r="G66">
+        <f t="shared" si="5"/>
         <v>99</v>
       </c>
-      <c r="G66">
-        <f t="shared" si="5"/>
-        <v>255</v>
-      </c>
       <c r="H66">
         <f t="shared" si="6"/>
-        <v>373</v>
+        <v>118</v>
       </c>
       <c r="I66" t="str">
         <f t="shared" si="7"/>
@@ -3651,7 +3651,7 @@
       </c>
       <c r="K66" t="str">
         <f t="shared" si="9"/>
-        <v>{"background": "#1363FF", "foreground": "#FFFFFF"}</v>
+        <v>{"background": "#001363", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -3660,43 +3660,43 @@
       </c>
       <c r="B67" t="str">
         <f t="shared" ref="B67:B106" si="10">MID(A67,1,2)</f>
-        <v>82</v>
+        <v>00</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C106" si="11">MID(A67,3,2)</f>
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" ref="D67:D106" si="12">MID(A67,5,2)</f>
-        <v>FF</v>
+        <v>72</v>
       </c>
       <c r="E67">
         <f t="shared" ref="E67:E106" si="13">HEX2DEC(B67)</f>
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="F67">
         <f t="shared" ref="F67:F106" si="14">HEX2DEC(C67)</f>
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="G67">
         <f t="shared" ref="G67:G106" si="15">HEX2DEC(D67)</f>
-        <v>255</v>
+        <v>114</v>
       </c>
       <c r="H67">
         <f t="shared" ref="H67:H106" si="16">SUM(E67:G67)</f>
-        <v>499</v>
+        <v>244</v>
       </c>
       <c r="I67" t="str">
         <f t="shared" ref="I67:I106" si="17">IF(H67&gt;382,"light","dark")</f>
-        <v>light</v>
+        <v>dark</v>
       </c>
       <c r="J67" t="str">
         <f t="shared" ref="J67:J106" si="18">IF(H67&gt;382,"000000","FFFFFF")</f>
-        <v>000000</v>
+        <v>FFFFFF</v>
       </c>
       <c r="K67" t="str">
         <f t="shared" ref="K67:K106" si="19">SUBSTITUTE(_xlfn.CONCAT("{'background': '#",A67,"', 'foreground': '#",J67,"'}"),"'","""")</f>
-        <v>{"background": "#8272FF", "foreground": "#000000"}</v>
+        <v>{"background": "#008272", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -3750,43 +3750,43 @@
       </c>
       <c r="B69" t="str">
         <f t="shared" si="10"/>
-        <v>73</v>
+        <v>00</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="11"/>
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="12"/>
-        <v>FF</v>
+        <v>65</v>
       </c>
       <c r="E69">
         <f t="shared" si="13"/>
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="F69">
         <f t="shared" si="14"/>
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="G69">
         <f t="shared" si="15"/>
-        <v>255</v>
+        <v>101</v>
       </c>
       <c r="H69">
         <f t="shared" si="16"/>
-        <v>471</v>
+        <v>216</v>
       </c>
       <c r="I69" t="str">
         <f t="shared" si="17"/>
-        <v>light</v>
+        <v>dark</v>
       </c>
       <c r="J69" t="str">
         <f t="shared" si="18"/>
-        <v>000000</v>
+        <v>FFFFFF</v>
       </c>
       <c r="K69" t="str">
         <f t="shared" si="19"/>
-        <v>{"background": "#7365FF", "foreground": "#000000"}</v>
+        <v>{"background": "#007365", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -3795,43 +3795,43 @@
       </c>
       <c r="B70" t="str">
         <f t="shared" si="10"/>
-        <v>58</v>
+        <v>00</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="12"/>
-        <v>FF</v>
+        <v>50</v>
       </c>
       <c r="E70">
         <f t="shared" si="13"/>
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="F70">
         <f t="shared" si="14"/>
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="G70">
         <f t="shared" si="15"/>
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="H70">
         <f t="shared" si="16"/>
-        <v>423</v>
+        <v>168</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" si="17"/>
-        <v>light</v>
+        <v>dark</v>
       </c>
       <c r="J70" t="str">
         <f t="shared" si="18"/>
-        <v>000000</v>
+        <v>FFFFFF</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="19"/>
-        <v>{"background": "#5850FF", "foreground": "#000000"}</v>
+        <v>{"background": "#005850", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -3975,43 +3975,43 @@
       </c>
       <c r="B74" t="str">
         <f t="shared" si="10"/>
-        <v>87</v>
+        <v>00</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="11"/>
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="12"/>
-        <v>FF</v>
+        <v>70</v>
       </c>
       <c r="E74">
         <f t="shared" si="13"/>
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="F74">
         <f t="shared" si="14"/>
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="G74">
         <f t="shared" si="15"/>
-        <v>255</v>
+        <v>112</v>
       </c>
       <c r="H74">
         <f t="shared" si="16"/>
-        <v>502</v>
+        <v>247</v>
       </c>
       <c r="I74" t="str">
         <f t="shared" si="17"/>
-        <v>light</v>
+        <v>dark</v>
       </c>
       <c r="J74" t="str">
         <f t="shared" si="18"/>
-        <v>000000</v>
+        <v>FFFFFF</v>
       </c>
       <c r="K74" t="str">
         <f t="shared" si="19"/>
-        <v>{"background": "#8770FF", "foreground": "#000000"}</v>
+        <v>{"background": "#008770", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -5457,5 +5457,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A65" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed footer not to be sticky, removed duplicate color
</commit_message>
<xml_diff>
--- a/src/assets/colors.xlsx
+++ b/src/assets/colors.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cherrw\Dropbox\Code\vsimages\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chryw\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8958"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
   <si>
     <t>FFF200</t>
   </si>
@@ -683,18 +683,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.15625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>89</v>
       </c>
@@ -729,7 +729,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -774,7 +774,7 @@
         <v>{"background": "#FFF200", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -819,7 +819,7 @@
         <v>{"background": "#FFF100", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -864,7 +864,7 @@
         <v>{"background": "#FFF880", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -909,7 +909,7 @@
         <v>{"background": "#F0E300", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -954,7 +954,7 @@
         <v>{"background": "#CCC000", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -999,7 +999,7 @@
         <v>{"background": "#FFB900", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>{"background": "#FFCB40", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>{"background": "#F0AE00", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>{"background": "#C78E00", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>{"background": "#FF8C00", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>{"background": "#FFA940", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>{"background": "#F08400", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>{"background": "#BA6800", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>{"background": "#D83B01", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>{"background": "#E26C41", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>{"background": "#BD3604", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>{"background": "#9C2801", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>{"background": "#E81123", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>{"background": "#EE4D5A", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>{"background": "#D91021", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>{"background": "#A3111E", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>{"background": "#A80000", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>{"background": "#BE4040", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
         <v>990000</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>{"background": "#990000", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3">
         <v>750000</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>{"background": "#750000", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>{"background": "#B4009E", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>{"background": "#C740B6", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>{"background": "#9E008B", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3">
         <v>850063</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>{"background": "#850063", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="s">
         <v>26</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>{"background": "#E3008C", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3" t="s">
         <v>27</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>{"background": "#EA40A9", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="s">
         <v>28</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>{"background": "#D40083", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3" t="s">
         <v>29</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>{"background": "#9C005F", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>{"background": "#5C005C", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3">
         <v>854085</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>{"background": "#854085", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3" t="s">
         <v>31</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>{"background": "#4D004D", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3">
         <v>380038</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>{"background": "#380038", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3" t="s">
         <v>32</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>{"background": "#5C2D91", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="s">
         <v>33</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>{"background": "#8562AD", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3">
         <v>522882</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>{"background": "#522882", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3">
         <v>401467</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>{"background": "#401467", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3" t="s">
         <v>34</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>{"background": "#B4A0FF", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3" t="s">
         <v>35</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>{"background": "#C7B8FF", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
         <v>36</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>{"background": "#A996F0", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3" t="s">
         <v>37</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>{"background": "#9080CF", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3" t="s">
         <v>38</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>{"background": "#32145A", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3" t="s">
         <v>39</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>{"background": "#654F83", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3" t="s">
         <v>40</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>{"background": "#28114A", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3" t="s">
         <v>41</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>{"background": "#220C3D", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3" t="s">
         <v>42</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>{"background": "#0078D7", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3" t="s">
         <v>43</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>{"background": "#409AE1", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3" t="s">
         <v>44</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>{"background": "#006FC8", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3" t="s">
         <v>90</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>{"background": "#5291FF", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="3" t="s">
         <v>45</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>{"background": "#00BCF2", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="3" t="s">
         <v>46</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>{"background": "#40CDF5", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3" t="s">
         <v>47</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>{"background": "#00B0E3", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3" t="s">
         <v>48</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>{"background": "#0086AD", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3" t="s">
         <v>91</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>{"background": "#2050FF", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="3" t="s">
         <v>49</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>{"background": "#40587C", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="3" t="s">
         <v>50</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>{"background": "#001A41", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="3" t="s">
         <v>92</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>{"background": "#1129FF", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="3" t="s">
         <v>51</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>{"background": "#00188F", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3" t="s">
         <v>52</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>{"background": "#4052AB", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3" t="s">
         <v>93</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>{"background": "#001580", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="3" t="s">
         <v>94</v>
       </c>
@@ -3654,52 +3654,52 @@
         <v>{"background": "#001363", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B106" si="10">MID(A67,1,2)</f>
+        <f t="shared" ref="B67:B105" si="10">MID(A67,1,2)</f>
         <v>00</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" ref="C67:C106" si="11">MID(A67,3,2)</f>
+        <f t="shared" ref="C67:C105" si="11">MID(A67,3,2)</f>
         <v>82</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D106" si="12">MID(A67,5,2)</f>
+        <f t="shared" ref="D67:D105" si="12">MID(A67,5,2)</f>
         <v>72</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E106" si="13">HEX2DEC(B67)</f>
+        <f t="shared" ref="E67:E105" si="13">HEX2DEC(B67)</f>
         <v>0</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F106" si="14">HEX2DEC(C67)</f>
+        <f t="shared" ref="F67:F105" si="14">HEX2DEC(C67)</f>
         <v>130</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G106" si="15">HEX2DEC(D67)</f>
+        <f t="shared" ref="G67:G105" si="15">HEX2DEC(D67)</f>
         <v>114</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H106" si="16">SUM(E67:G67)</f>
+        <f t="shared" ref="H67:H105" si="16">SUM(E67:G67)</f>
         <v>244</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67:I106" si="17">IF(H67&gt;382,"light","dark")</f>
+        <f t="shared" ref="I67:I105" si="17">IF(H67&gt;382,"light","dark")</f>
         <v>dark</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J106" si="18">IF(H67&gt;382,"000000","FFFFFF")</f>
+        <f t="shared" ref="J67:J105" si="18">IF(H67&gt;382,"000000","FFFFFF")</f>
         <v>FFFFFF</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" ref="K67:K106" si="19">SUBSTITUTE(_xlfn.CONCAT("{'background': '#",A67,"', 'foreground': '#",J67,"'}"),"'","""")</f>
+        <f t="shared" ref="K67:K105" si="19">SUBSTITUTE(_xlfn.CONCAT("{'background': '#",A67,"', 'foreground': '#",J67,"'}"),"'","""")</f>
         <v>{"background": "#008272", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="3" t="s">
         <v>53</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>{"background": "#40A195", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="3" t="s">
         <v>96</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>{"background": "#007365", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="3" t="s">
         <v>97</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>{"background": "#005850", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="3" t="s">
         <v>54</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>{"background": "#00B294", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="3" t="s">
         <v>55</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>{"background": "#40C5AF", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3" t="s">
         <v>56</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>{"background": "#00A387", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="3" t="s">
         <v>98</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>{"background": "#008770", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="3" t="s">
         <v>57</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>{"background": "#004B50", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="3" t="s">
         <v>58</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>{"background": "#40787C", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="3" t="s">
         <v>59</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>{"background": "#003D41", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="3" t="s">
         <v>60</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>{"background": "#002F33", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="3" t="s">
         <v>61</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>{"background": "#107C10", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="3" t="s">
         <v>62</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>{"background": "#4C9D4C", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="3" t="s">
         <v>63</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>{"background": "#0E6D0E", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="3">
         <v>106110</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>{"background": "#106110", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="3" t="s">
         <v>64</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>{"background": "#BAD80A", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="3" t="s">
         <v>65</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>{"background": "#CBE247", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="3" t="s">
         <v>66</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>{"background": "#ADC909", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="3" t="s">
         <v>67</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>{"background": "#91A80A", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="3" t="s">
         <v>68</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>{"background": "#004B1C", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="3">
         <v>407855</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>{"background": "#407855", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="3" t="s">
         <v>69</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>{"background": "#003C16", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="3" t="s">
         <v>70</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>{"background": "#00240D", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="3">
         <v>505050</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>{"background": "#505050", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="3">
         <v>282828</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>{"background": "#282828", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="3" t="s">
         <v>71</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>{"background": "#D2D2D2", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="3" t="s">
         <v>72</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>{"background": "#F3F3F3", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="3" t="s">
         <v>73</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>{"background": "#E6E6E6", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="3">
         <v>939393</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>{"background": "#939393", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="3">
         <v>737373</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>{"background": "#737373", "foreground": "#FFFFFF"}</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="3" t="s">
         <v>74</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>{"background": "#C2C2C2", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="3" t="s">
         <v>75</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>{"background": "#B2B2B2", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="3" t="s">
         <v>76</v>
       </c>
@@ -5184,127 +5184,127 @@
         <v>{"background": "#FFFFFF", "foreground": "#000000"}</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B101" t="str">
         <f t="shared" si="10"/>
-        <v>E6</v>
+        <v>8E</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="11"/>
-        <v>E6</v>
+        <v>56</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="12"/>
-        <v>E6</v>
+        <v>2E</v>
       </c>
       <c r="E101">
         <f t="shared" si="13"/>
-        <v>230</v>
+        <v>142</v>
       </c>
       <c r="F101">
         <f t="shared" si="14"/>
-        <v>230</v>
+        <v>86</v>
       </c>
       <c r="G101">
         <f t="shared" si="15"/>
-        <v>230</v>
+        <v>46</v>
       </c>
       <c r="H101">
         <f t="shared" si="16"/>
-        <v>690</v>
+        <v>274</v>
       </c>
       <c r="I101" t="str">
         <f t="shared" si="17"/>
-        <v>light</v>
+        <v>dark</v>
       </c>
       <c r="J101" t="str">
         <f t="shared" si="18"/>
-        <v>000000</v>
+        <v>FFFFFF</v>
       </c>
       <c r="K101" t="str">
         <f t="shared" si="19"/>
-        <v>{"background": "#E6E6E6", "foreground": "#000000"}</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+        <v>{"background": "#8E562E", "foreground": "#FFFFFF"}</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B102" t="str">
         <f t="shared" si="10"/>
-        <v>8E</v>
+        <v>D8</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="11"/>
-        <v>56</v>
+        <v>B0</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="12"/>
-        <v>2E</v>
+        <v>94</v>
       </c>
       <c r="E102">
         <f t="shared" si="13"/>
-        <v>142</v>
+        <v>216</v>
       </c>
       <c r="F102">
         <f t="shared" si="14"/>
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="G102">
         <f t="shared" si="15"/>
-        <v>46</v>
+        <v>148</v>
       </c>
       <c r="H102">
         <f t="shared" si="16"/>
-        <v>274</v>
+        <v>540</v>
       </c>
       <c r="I102" t="str">
         <f t="shared" si="17"/>
-        <v>dark</v>
+        <v>light</v>
       </c>
       <c r="J102" t="str">
         <f t="shared" si="18"/>
-        <v>FFFFFF</v>
+        <v>000000</v>
       </c>
       <c r="K102" t="str">
         <f t="shared" si="19"/>
-        <v>{"background": "#8E562E", "foreground": "#FFFFFF"}</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+        <v>{"background": "#D8B094", "foreground": "#000000"}</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B103" t="str">
         <f t="shared" si="10"/>
-        <v>D8</v>
+        <v>BB</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="11"/>
-        <v>B0</v>
+        <v>91</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="12"/>
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="E103">
         <f t="shared" si="13"/>
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="F103">
         <f t="shared" si="14"/>
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="G103">
         <f t="shared" si="15"/>
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="H103">
         <f t="shared" si="16"/>
-        <v>540</v>
+        <v>435</v>
       </c>
       <c r="I103" t="str">
         <f t="shared" si="17"/>
@@ -5316,140 +5316,95 @@
       </c>
       <c r="K103" t="str">
         <f t="shared" si="19"/>
-        <v>{"background": "#D8B094", "foreground": "#000000"}</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+        <v>{"background": "#BB9167", "foreground": "#000000"}</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B104" t="str">
         <f t="shared" si="10"/>
-        <v>BB</v>
+        <v>61</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="11"/>
-        <v>91</v>
+        <v>3D</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="12"/>
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="E104">
         <f t="shared" si="13"/>
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="F104">
         <f t="shared" si="14"/>
-        <v>145</v>
+        <v>61</v>
       </c>
       <c r="G104">
         <f t="shared" si="15"/>
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="H104">
         <f t="shared" si="16"/>
-        <v>435</v>
+        <v>206</v>
       </c>
       <c r="I104" t="str">
         <f t="shared" si="17"/>
-        <v>light</v>
+        <v>dark</v>
       </c>
       <c r="J104" t="str">
         <f t="shared" si="18"/>
-        <v>000000</v>
+        <v>FFFFFF</v>
       </c>
       <c r="K104" t="str">
         <f t="shared" si="19"/>
-        <v>{"background": "#BB9167", "foreground": "#000000"}</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+        <v>{"background": "#613D30", "foreground": "#FFFFFF"}</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B105" t="str">
         <f t="shared" si="10"/>
-        <v>61</v>
+        <v>F7</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="11"/>
-        <v>3D</v>
+        <v>D7</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="12"/>
-        <v>30</v>
+        <v>C4</v>
       </c>
       <c r="E105">
         <f t="shared" si="13"/>
-        <v>97</v>
+        <v>247</v>
       </c>
       <c r="F105">
         <f t="shared" si="14"/>
-        <v>61</v>
+        <v>215</v>
       </c>
       <c r="G105">
         <f t="shared" si="15"/>
-        <v>48</v>
+        <v>196</v>
       </c>
       <c r="H105">
         <f t="shared" si="16"/>
-        <v>206</v>
+        <v>658</v>
       </c>
       <c r="I105" t="str">
         <f t="shared" si="17"/>
-        <v>dark</v>
+        <v>light</v>
       </c>
       <c r="J105" t="str">
         <f t="shared" si="18"/>
-        <v>FFFFFF</v>
+        <v>000000</v>
       </c>
       <c r="K105" t="str">
-        <f t="shared" si="19"/>
-        <v>{"background": "#613D30", "foreground": "#FFFFFF"}</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B106" t="str">
-        <f t="shared" si="10"/>
-        <v>F7</v>
-      </c>
-      <c r="C106" t="str">
-        <f t="shared" si="11"/>
-        <v>D7</v>
-      </c>
-      <c r="D106" t="str">
-        <f t="shared" si="12"/>
-        <v>C4</v>
-      </c>
-      <c r="E106">
-        <f t="shared" si="13"/>
-        <v>247</v>
-      </c>
-      <c r="F106">
-        <f t="shared" si="14"/>
-        <v>215</v>
-      </c>
-      <c r="G106">
-        <f t="shared" si="15"/>
-        <v>196</v>
-      </c>
-      <c r="H106">
-        <f t="shared" si="16"/>
-        <v>658</v>
-      </c>
-      <c r="I106" t="str">
-        <f t="shared" si="17"/>
-        <v>light</v>
-      </c>
-      <c r="J106" t="str">
-        <f t="shared" si="18"/>
-        <v>000000</v>
-      </c>
-      <c r="K106" t="str">
         <f t="shared" si="19"/>
         <v>{"background": "#F7D7C4", "foreground": "#000000"}</v>
       </c>

</xml_diff>